<commit_message>
Sliced remaining files and added hardware list.
</commit_message>
<xml_diff>
--- a/CADandPCB/robotArm/Part-Tracker.xlsx
+++ b/CADandPCB/robotArm/Part-Tracker.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Sherstan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MarkSherstan/Documents/GitHub Projects/GestureControlledRoboticArm_MecE653/CADandPCB/robotArm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7607C5AF-225D-493E-85E0-4B671E4AD4EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701AE44C-F7AC-C043-86BD-6BFE6AA40A54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="2175" windowWidth="28800" windowHeight="11385" xr2:uid="{F5457483-B9A6-4FDD-8E51-56CF0918A53C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{F5457483-B9A6-4FDD-8E51-56CF0918A53C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Printing" sheetId="1" r:id="rId1"/>
+    <sheet name="Hardware" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Printing!$A$1:$J$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
   <si>
     <t>EBAmk2_001_base.STL</t>
   </si>
@@ -160,6 +160,117 @@
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t>EBAmk2_012_mainbase_NEW</t>
+  </si>
+  <si>
+    <t>Claw</t>
+  </si>
+  <si>
+    <t>Added 3 walls</t>
+  </si>
+  <si>
+    <t>Gears</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>EBAmk2_013_lower_base</t>
+  </si>
+  <si>
+    <t>Speed MK3</t>
+  </si>
+  <si>
+    <t>Joints</t>
+  </si>
+  <si>
+    <t>4 wall + supports</t>
+  </si>
+  <si>
+    <t>horarm</t>
+  </si>
+  <si>
+    <t>Arms</t>
+  </si>
+  <si>
+    <t>M4 Washers</t>
+  </si>
+  <si>
+    <t>955 or 946 servo </t>
+  </si>
+  <si>
+    <t>SG90 SERVO </t>
+  </si>
+  <si>
+    <t>M6 selflocking nut </t>
+  </si>
+  <si>
+    <t>M6x25 screw </t>
+  </si>
+  <si>
+    <t>M3 selflocking nuts </t>
+  </si>
+  <si>
+    <t>M3 x 20 screws </t>
+  </si>
+  <si>
+    <t>M3 x 10 hex recessed head screw </t>
+  </si>
+  <si>
+    <t>M4 selflocking nuts </t>
+  </si>
+  <si>
+    <t>M4 x 40 screw </t>
+  </si>
+  <si>
+    <t>M4 x 30 screw </t>
+  </si>
+  <si>
+    <t>M4 x 20 screw </t>
+  </si>
+  <si>
+    <t>M4 x 60mm threaded rod </t>
+  </si>
+  <si>
+    <t>M4 x 32mm threaded rod </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dia 6 mm ball spheres </t>
+  </si>
+  <si>
+    <t>606zz bearing </t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>RPI Shield?</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Voltage Regulator</t>
+  </si>
+  <si>
+    <t>Power supply or LiPo Battery</t>
+  </si>
+  <si>
+    <t>Double check bolt pattern</t>
+  </si>
+  <si>
+    <t>Ordered 608zz</t>
+  </si>
+  <si>
+    <t>Ordered 1/4"</t>
   </si>
 </sst>
 </file>
@@ -167,10 +278,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="174" formatCode="0.0%"/>
-    <numFmt numFmtId="175" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,8 +328,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +345,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,11 +440,22 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -329,27 +463,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <strike/>
@@ -667,23 +781,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012563A3-52C3-4EE8-8704-0D1DE9BE504A}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="20">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -715,7 +831,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,48 +860,75 @@
       <c r="I2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="12"/>
+      <c r="J2" s="12">
+        <v>43512</v>
+      </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>56</v>
+      </c>
       <c r="E3" s="13">
         <f t="shared" ref="E3:E23" si="0">IFERROR((B3)+(C3/60)+(D3/3600),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="13"/>
+        <v>6.5488888888888885</v>
+      </c>
+      <c r="F3" s="13">
+        <v>67.319999999999993</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="13"/>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -814,9 +957,11 @@
       <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J5" s="12">
+        <v>43512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -845,28 +990,42 @@
       <c r="I6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="12">
+        <v>43512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4">
+        <v>11</v>
+      </c>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="13"/>
+        <v>5.2697222222222218</v>
+      </c>
+      <c r="F7" s="13">
+        <v>49.04</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -881,30 +1040,44 @@
       <c r="G8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4">
+        <v>49</v>
+      </c>
       <c r="E9" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="13"/>
+        <v>3.6136111111111111</v>
+      </c>
+      <c r="F9" s="13">
+        <v>29.5</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -933,142 +1106,226 @@
       <c r="I10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="12">
+        <v>43512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="13"/>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4">
+        <v>58</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12</v>
+      </c>
       <c r="E12" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="13"/>
+        <v>2.97</v>
+      </c>
+      <c r="F12" s="13">
+        <v>29.1</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="13"/>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="13"/>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="13"/>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="4">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44</v>
+      </c>
       <c r="E16" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="13"/>
+        <v>13.078888888888889</v>
+      </c>
+      <c r="F16" s="13">
+        <v>139.55000000000001</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>55</v>
+      </c>
+      <c r="D17" s="4">
+        <v>33</v>
+      </c>
       <c r="E17" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="13"/>
+        <v>1.9258333333333333</v>
+      </c>
+      <c r="F17" s="13">
+        <v>25.45</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1095,85 +1352,143 @@
         <v>32</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="12">
+        <v>43512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>42</v>
+      </c>
+      <c r="D19" s="4">
+        <v>23</v>
+      </c>
       <c r="E19" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="13"/>
+        <v>0.70638888888888884</v>
+      </c>
+      <c r="F19" s="13">
+        <v>5.32</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="12">
+        <v>43513</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="13"/>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="12">
+        <v>43513</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="13"/>
+      <c r="B21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="12">
+        <v>43513</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="13"/>
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="12">
+        <v>43513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1519,7 @@
         <v>43512</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="16" thickBot="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1216,7 +1531,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="17" thickBot="1">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="8" t="s">
@@ -1224,11 +1539,11 @@
       </c>
       <c r="E25" s="9" t="str">
         <f>ROUND(SUM(E2:E23),1) &amp; " h"</f>
-        <v>12.1 h</v>
+        <v>46.2 h</v>
       </c>
       <c r="F25" s="10" t="str">
         <f>ROUND(SUM(F2:F23),1) &amp; " g"</f>
-        <v>125.3 g</v>
+        <v>470.6 g</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -1237,16 +1552,222 @@
       </c>
       <c r="J25" s="11">
         <f>SUMIF(J2:J23,"&gt;1",E2:E23)/SUM(E2:E23)</f>
-        <v>0.11136906951084956</v>
+        <v>0.27687118187503007</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J23" xr:uid="{EC696274-73D5-4FA2-AB63-3A381666B3CA}"/>
   <conditionalFormatting sqref="A2:I23">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$J2&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336E3C69-C2C7-E946-9804-CFC829250AB4}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19">
+      <c r="A1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="16">
+        <v>3</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="16">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="16">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="16">
+        <v>2</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="16">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="16">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="16">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="16">
+        <v>5</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="16">
+        <v>1</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="16">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="16">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="16">
+        <v>20</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="19">
+      <c r="A19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="16">
+        <v>1</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="16">
+        <v>1</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="16">
+        <v>1</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated part tracker with all printing.
</commit_message>
<xml_diff>
--- a/CADandPCB/robotArm/Part-Tracker.xlsx
+++ b/CADandPCB/robotArm/Part-Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Sherstan\Documents\GitHub Projects\GestureControlledRoboticArm_MecE653\CADandPCB\robotArm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D81C16E-A668-4DB0-B5B0-65565B82CEAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7338A004-2518-4556-8758-3A65FF0CF557}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5820" yWindow="2700" windowWidth="11835" windowHeight="10725" xr2:uid="{F5457483-B9A6-4FDD-8E51-56CF0918A53C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{F5457483-B9A6-4FDD-8E51-56CF0918A53C}"/>
   </bookViews>
   <sheets>
     <sheet name="Printing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
   <si>
     <t>EBAmk2_001_base.STL</t>
   </si>
@@ -272,9 +272,6 @@
   </si>
   <si>
     <t>Modified_EBAmk2_013_lower_base</t>
-  </si>
-  <si>
-    <t>Increased for 608 zz bearing</t>
   </si>
 </sst>
 </file>
@@ -453,10 +450,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012563A3-52C3-4EE8-8704-0D1DE9BE504A}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1024,9 @@
       <c r="I7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="12">
+        <v>43514</v>
+      </c>
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1306,7 +1305,7 @@
       <c r="I16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="18">
         <v>43514</v>
       </c>
     </row>
@@ -1339,10 +1338,10 @@
       <c r="I17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="J17" s="12">
+        <v>43514</v>
+      </c>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1571,7 +1570,7 @@
       </c>
       <c r="J25" s="11">
         <f>SUMIF(J2:J23,"&gt;1",E2:E23)/SUM(E2:E23)</f>
-        <v>0.84442733767952083</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1589,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336E3C69-C2C7-E946-9804-CFC829250AB4}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,11 +1752,11 @@
       <c r="A18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
@@ -1788,5 +1787,6 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>